<commit_message>
fix bugs in index.html
</commit_message>
<xml_diff>
--- a/test/IntegrationTest_Index.xlsx
+++ b/test/IntegrationTest_Index.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="78">
   <si>
     <t>design</t>
   </si>
@@ -266,11 +266,10 @@
     <t>1. open from the mobile or inspection on the pc</t>
   </si>
   <si>
-    <t>- "Contact Us" of footer should be one line
-'- Search button should be one line with search bar like Firefox</t>
+    <t>"Contact Us" of footer should be one line</t>
   </si>
   <si>
-    <t>"Contact Us" of footer should be one line</t>
+    <t>Search button should be one line with search bar like Firefox</t>
   </si>
 </sst>
 </file>
@@ -402,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -446,6 +445,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -455,20 +460,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -683,76 +688,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1185,13 +1120,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1252,13 +1187,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1284,9 +1219,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1310,9 +1245,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1336,9 +1271,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1362,9 +1297,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1388,9 +1323,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1416,9 +1351,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1442,9 +1377,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1468,11 +1403,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
@@ -1496,9 +1431,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1522,9 +1457,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1548,9 +1483,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1574,11 +1509,11 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1604,9 +1539,9 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -1630,9 +1565,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1658,9 +1593,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1684,9 +1619,9 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1712,9 +1647,9 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -1740,9 +1675,9 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -1764,9 +1699,9 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -1786,9 +1721,9 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -1814,9 +1749,9 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -1840,9 +1775,9 @@
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1868,9 +1803,9 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -1896,13 +1831,13 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="22" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1928,9 +1863,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1954,9 +1889,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="4" t="s">
         <v>13</v>
       </c>
@@ -1980,9 +1915,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="4" t="s">
         <v>14</v>
       </c>
@@ -2006,9 +1941,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
@@ -2032,9 +1967,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -2060,9 +1995,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="4" t="s">
         <v>20</v>
       </c>
@@ -2086,9 +2021,9 @@
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="4" t="s">
         <v>21</v>
       </c>
@@ -2112,11 +2047,11 @@
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="21"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="4" t="s">
         <v>24</v>
       </c>
@@ -2140,9 +2075,9 @@
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="4" t="s">
         <v>26</v>
       </c>
@@ -2166,9 +2101,9 @@
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="4" t="s">
         <v>28</v>
       </c>
@@ -2192,9 +2127,9 @@
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="4" t="s">
         <v>30</v>
       </c>
@@ -2214,27 +2149,27 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21" t="s">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="23" t="s">
         <v>33</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="17" t="s">
         <v>76</v>
       </c>
       <c r="I38" s="3">
@@ -2243,28 +2178,24 @@
       <c r="J38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="7">
-        <v>38</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="K38" s="3">
+        <v>42871</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
       <c r="G39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="17" t="s">
         <v>77</v>
       </c>
       <c r="I39" s="3">
@@ -2276,13 +2207,44 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
+    <row r="40" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="3">
+        <v>42871</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="3">
+        <v>42871</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
+  <mergeCells count="19">
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
     <mergeCell ref="D26:D30"/>
     <mergeCell ref="D31:D33"/>
     <mergeCell ref="D34:D37"/>
@@ -2290,12 +2252,18 @@
     <mergeCell ref="C14:C25"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C2:C9"/>
-    <mergeCell ref="B26:B39"/>
+    <mergeCell ref="B26:B40"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:L39">
+  <conditionalFormatting sqref="E2:L38 E40:L40 G39:L39">
     <cfRule type="expression" dxfId="30" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
@@ -2307,7 +2275,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G40">
       <formula1>"OK, NG"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2382,13 +2350,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -2408,9 +2376,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -2428,9 +2396,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -2448,9 +2416,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -2468,9 +2436,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -2488,9 +2456,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -2510,9 +2478,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -2530,9 +2498,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -2550,11 +2518,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -2572,9 +2540,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2592,9 +2560,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -2612,9 +2580,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -2632,11 +2600,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -2662,9 +2630,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -2688,9 +2656,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -2714,9 +2682,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2740,9 +2708,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -2766,9 +2734,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -2792,9 +2760,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -2814,9 +2782,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -2834,9 +2802,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -2854,9 +2822,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -2874,9 +2842,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -2894,9 +2862,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -2914,13 +2882,13 @@
       <c r="A26" s="7">
         <v>29</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -2940,9 +2908,9 @@
       <c r="A27" s="7">
         <v>30</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
@@ -2960,9 +2928,9 @@
       <c r="A28" s="7">
         <v>31</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
@@ -2980,9 +2948,9 @@
       <c r="A29" s="7">
         <v>32</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="10" t="s">
         <v>14</v>
       </c>
@@ -3000,9 +2968,9 @@
       <c r="A30" s="7">
         <v>33</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
@@ -3020,9 +2988,9 @@
       <c r="A31" s="7">
         <v>34</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -3042,9 +3010,9 @@
       <c r="A32" s="7">
         <v>35</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="10" t="s">
         <v>20</v>
       </c>
@@ -3062,9 +3030,9 @@
       <c r="A33" s="7">
         <v>36</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="10" t="s">
         <v>21</v>
       </c>
@@ -3082,11 +3050,11 @@
       <c r="A34" s="7">
         <v>37</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="10" t="s">
         <v>24</v>
       </c>
@@ -3104,9 +3072,9 @@
       <c r="A35" s="7">
         <v>38</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="10" t="s">
         <v>26</v>
       </c>
@@ -3124,9 +3092,9 @@
       <c r="A36" s="7">
         <v>39</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="10" t="s">
         <v>28</v>
       </c>
@@ -3144,9 +3112,9 @@
       <c r="A37" s="7">
         <v>40</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="10" t="s">
         <v>30</v>
       </c>
@@ -3164,11 +3132,11 @@
       <c r="A38" s="7">
         <v>41</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -3194,9 +3162,9 @@
       <c r="A39" s="7">
         <v>42</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
         <v>45</v>
       </c>
@@ -3220,9 +3188,9 @@
       <c r="A40" s="7">
         <v>43</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="4" t="s">
         <v>42</v>
       </c>
@@ -3246,9 +3214,9 @@
       <c r="A41" s="7">
         <v>44</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
         <v>43</v>
       </c>
@@ -3272,9 +3240,9 @@
       <c r="A42" s="7">
         <v>45</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="4" t="s">
         <v>46</v>
       </c>
@@ -3298,9 +3266,9 @@
       <c r="A43" s="7">
         <v>46</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
@@ -3324,9 +3292,9 @@
       <c r="A44" s="7">
         <v>47</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="17" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -3346,9 +3314,9 @@
       <c r="A45" s="7">
         <v>48</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
         <v>45</v>
       </c>
@@ -3366,9 +3334,9 @@
       <c r="A46" s="7">
         <v>49</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
@@ -3386,9 +3354,9 @@
       <c r="A47" s="7">
         <v>50</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
@@ -3406,9 +3374,9 @@
       <c r="A48" s="7">
         <v>51</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>46</v>
       </c>
@@ -3426,9 +3394,9 @@
       <c r="A49" s="7">
         <v>52</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="4" t="s">
         <v>44</v>
       </c>
@@ -3444,6 +3412,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:B49"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -3453,15 +3430,6 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B26:B49"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="27" priority="7">
@@ -3558,13 +3526,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -3584,9 +3552,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -3604,9 +3572,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -3624,9 +3592,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -3644,9 +3612,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -3664,9 +3632,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -3686,9 +3654,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -3706,9 +3674,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -3726,11 +3694,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -3748,9 +3716,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -3768,9 +3736,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -3788,9 +3756,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -3808,11 +3776,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -3832,9 +3800,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -3852,9 +3820,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -3872,9 +3840,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -3892,9 +3860,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -3912,9 +3880,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -3932,9 +3900,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -3954,9 +3922,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -3974,9 +3942,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -3994,9 +3962,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -4014,9 +3982,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -4034,9 +4002,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -4054,13 +4022,13 @@
       <c r="A26" s="7">
         <v>29</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -4080,9 +4048,9 @@
       <c r="A27" s="7">
         <v>30</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
@@ -4100,9 +4068,9 @@
       <c r="A28" s="7">
         <v>31</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
@@ -4120,9 +4088,9 @@
       <c r="A29" s="7">
         <v>32</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="10" t="s">
         <v>14</v>
       </c>
@@ -4140,9 +4108,9 @@
       <c r="A30" s="7">
         <v>33</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
@@ -4160,9 +4128,9 @@
       <c r="A31" s="7">
         <v>34</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -4182,9 +4150,9 @@
       <c r="A32" s="7">
         <v>35</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="10" t="s">
         <v>20</v>
       </c>
@@ -4202,9 +4170,9 @@
       <c r="A33" s="7">
         <v>36</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="10" t="s">
         <v>21</v>
       </c>
@@ -4222,11 +4190,11 @@
       <c r="A34" s="7">
         <v>37</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="10" t="s">
         <v>24</v>
       </c>
@@ -4244,9 +4212,9 @@
       <c r="A35" s="7">
         <v>38</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="10" t="s">
         <v>26</v>
       </c>
@@ -4264,9 +4232,9 @@
       <c r="A36" s="7">
         <v>39</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="10" t="s">
         <v>28</v>
       </c>
@@ -4284,9 +4252,9 @@
       <c r="A37" s="7">
         <v>40</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="10" t="s">
         <v>30</v>
       </c>
@@ -4304,11 +4272,11 @@
       <c r="A38" s="7">
         <v>41</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -4328,9 +4296,9 @@
       <c r="A39" s="7">
         <v>42</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
         <v>45</v>
       </c>
@@ -4348,9 +4316,9 @@
       <c r="A40" s="7">
         <v>43</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="4" t="s">
         <v>42</v>
       </c>
@@ -4368,9 +4336,9 @@
       <c r="A41" s="7">
         <v>44</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
         <v>43</v>
       </c>
@@ -4388,9 +4356,9 @@
       <c r="A42" s="7">
         <v>45</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="4" t="s">
         <v>46</v>
       </c>
@@ -4408,9 +4376,9 @@
       <c r="A43" s="7">
         <v>46</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
@@ -4428,9 +4396,9 @@
       <c r="A44" s="7">
         <v>47</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="17" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -4450,9 +4418,9 @@
       <c r="A45" s="7">
         <v>48</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
         <v>45</v>
       </c>
@@ -4470,9 +4438,9 @@
       <c r="A46" s="7">
         <v>49</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
@@ -4490,9 +4458,9 @@
       <c r="A47" s="7">
         <v>50</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
@@ -4510,9 +4478,9 @@
       <c r="A48" s="7">
         <v>51</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>46</v>
       </c>
@@ -4530,9 +4498,9 @@
       <c r="A49" s="7">
         <v>52</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="4" t="s">
         <v>44</v>
       </c>
@@ -4548,6 +4516,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:B49"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -4557,15 +4534,6 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B26:B49"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="22" priority="5">
@@ -4662,13 +4630,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -4688,9 +4656,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -4708,9 +4676,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -4728,9 +4696,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -4748,9 +4716,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -4768,9 +4736,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -4790,9 +4758,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -4810,9 +4778,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -4830,11 +4798,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -4852,9 +4820,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -4872,9 +4840,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -4892,9 +4860,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -4912,9 +4880,9 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -4934,9 +4902,9 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="15" t="s">
         <v>67</v>
       </c>
@@ -4954,9 +4922,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="15" t="s">
         <v>68</v>
       </c>
@@ -4974,9 +4942,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="15" t="s">
         <v>69</v>
       </c>
@@ -4994,11 +4962,11 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -5018,9 +4986,9 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="4" t="s">
         <v>45</v>
       </c>
@@ -5038,9 +5006,9 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
@@ -5058,9 +5026,9 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>43</v>
       </c>
@@ -5078,9 +5046,9 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>46</v>
       </c>
@@ -5098,9 +5066,9 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="4" t="s">
         <v>44</v>
       </c>
@@ -5118,9 +5086,9 @@
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="17" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -5140,9 +5108,9 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
@@ -5160,9 +5128,9 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="4" t="s">
         <v>42</v>
       </c>
@@ -5180,9 +5148,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="4" t="s">
         <v>43</v>
       </c>
@@ -5200,9 +5168,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="4" t="s">
         <v>46</v>
       </c>
@@ -5220,9 +5188,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="4" t="s">
         <v>44</v>
       </c>
@@ -5240,13 +5208,13 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="10" t="s">
@@ -5266,9 +5234,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="10" t="s">
         <v>11</v>
       </c>
@@ -5286,9 +5254,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="10" t="s">
         <v>13</v>
       </c>
@@ -5306,9 +5274,9 @@
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="10" t="s">
         <v>14</v>
       </c>
@@ -5326,9 +5294,9 @@
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
       <c r="E34" s="10" t="s">
         <v>17</v>
       </c>
@@ -5346,9 +5314,9 @@
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="17" t="s">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="10" t="s">
@@ -5368,9 +5336,9 @@
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="10" t="s">
         <v>20</v>
       </c>
@@ -5388,9 +5356,9 @@
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="10" t="s">
         <v>21</v>
       </c>
@@ -5408,11 +5376,11 @@
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="17"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="10" t="s">
         <v>24</v>
       </c>
@@ -5430,9 +5398,9 @@
       <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="10" t="s">
         <v>26</v>
       </c>
@@ -5450,9 +5418,9 @@
       <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="10" t="s">
         <v>28</v>
       </c>
@@ -5470,9 +5438,9 @@
       <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
       <c r="E41" s="10" t="s">
         <v>30</v>
       </c>
@@ -5490,9 +5458,9 @@
       <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="17" t="s">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E42" s="13" t="s">
@@ -5512,9 +5480,9 @@
       <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
       <c r="E43" s="13" t="s">
         <v>67</v>
       </c>
@@ -5532,9 +5500,9 @@
       <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="13" t="s">
         <v>68</v>
       </c>
@@ -5552,9 +5520,9 @@
       <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
       <c r="E45" s="13" t="s">
         <v>69</v>
       </c>
@@ -5572,11 +5540,11 @@
       <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="17" t="s">
+      <c r="B46" s="20"/>
+      <c r="C46" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -5596,9 +5564,9 @@
       <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
         <v>45</v>
       </c>
@@ -5616,9 +5584,9 @@
       <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>42</v>
       </c>
@@ -5636,9 +5604,9 @@
       <c r="A49" s="7">
         <v>48</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
       <c r="E49" s="4" t="s">
         <v>43</v>
       </c>
@@ -5656,9 +5624,9 @@
       <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="4" t="s">
         <v>46</v>
       </c>
@@ -5676,9 +5644,9 @@
       <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="21"/>
       <c r="E51" s="4" t="s">
         <v>44</v>
       </c>
@@ -5696,9 +5664,9 @@
       <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="17" t="s">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="4" t="s">
@@ -5718,9 +5686,9 @@
       <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="4" t="s">
         <v>45</v>
       </c>
@@ -5738,9 +5706,9 @@
       <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
       <c r="E54" s="4" t="s">
         <v>42</v>
       </c>
@@ -5758,9 +5726,9 @@
       <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
       <c r="E55" s="4" t="s">
         <v>43</v>
       </c>
@@ -5778,9 +5746,9 @@
       <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
       <c r="E56" s="4" t="s">
         <v>46</v>
       </c>
@@ -5798,9 +5766,9 @@
       <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
       <c r="E57" s="4" t="s">
         <v>44</v>
       </c>
@@ -5816,6 +5784,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B30:B57"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C46:C57"/>
+    <mergeCell ref="D46:D51"/>
+    <mergeCell ref="D52:D57"/>
+    <mergeCell ref="C38:C45"/>
+    <mergeCell ref="D42:D45"/>
     <mergeCell ref="B2:B29"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -5826,16 +5804,6 @@
     <mergeCell ref="D24:D29"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="C10:C17"/>
-    <mergeCell ref="B30:B57"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C46:C57"/>
-    <mergeCell ref="D46:D51"/>
-    <mergeCell ref="D52:D57"/>
-    <mergeCell ref="C38:C45"/>
-    <mergeCell ref="D42:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D30 C38:D38 D52:D55 C46:D49 D35">
     <cfRule type="expression" dxfId="17" priority="5">
@@ -5943,13 +5911,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -5969,9 +5937,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -5989,9 +5957,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -6009,9 +5977,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -6029,9 +5997,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -6049,9 +6017,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -6071,9 +6039,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -6091,9 +6059,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -6111,11 +6079,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -6133,9 +6101,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -6153,9 +6121,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -6173,9 +6141,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -6193,11 +6161,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -6217,9 +6185,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -6237,9 +6205,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -6257,9 +6225,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -6277,9 +6245,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -6297,9 +6265,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -6317,9 +6285,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -6339,9 +6307,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -6359,9 +6327,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -6379,9 +6347,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -6399,9 +6367,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -6419,9 +6387,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -6439,13 +6407,13 @@
       <c r="A26" s="7">
         <v>29</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -6465,9 +6433,9 @@
       <c r="A27" s="7">
         <v>30</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
@@ -6485,9 +6453,9 @@
       <c r="A28" s="7">
         <v>31</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
@@ -6505,9 +6473,9 @@
       <c r="A29" s="7">
         <v>32</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="10" t="s">
         <v>14</v>
       </c>
@@ -6525,9 +6493,9 @@
       <c r="A30" s="7">
         <v>33</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
@@ -6545,9 +6513,9 @@
       <c r="A31" s="7">
         <v>34</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -6567,9 +6535,9 @@
       <c r="A32" s="7">
         <v>35</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="10" t="s">
         <v>20</v>
       </c>
@@ -6587,9 +6555,9 @@
       <c r="A33" s="7">
         <v>36</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="10" t="s">
         <v>21</v>
       </c>
@@ -6607,11 +6575,11 @@
       <c r="A34" s="7">
         <v>37</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="10" t="s">
         <v>24</v>
       </c>
@@ -6629,9 +6597,9 @@
       <c r="A35" s="7">
         <v>38</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="10" t="s">
         <v>26</v>
       </c>
@@ -6649,9 +6617,9 @@
       <c r="A36" s="7">
         <v>39</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="10" t="s">
         <v>28</v>
       </c>
@@ -6669,9 +6637,9 @@
       <c r="A37" s="7">
         <v>40</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="10" t="s">
         <v>30</v>
       </c>
@@ -6689,11 +6657,11 @@
       <c r="A38" s="7">
         <v>41</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -6713,9 +6681,9 @@
       <c r="A39" s="7">
         <v>42</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
         <v>45</v>
       </c>
@@ -6733,9 +6701,9 @@
       <c r="A40" s="7">
         <v>43</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="4" t="s">
         <v>42</v>
       </c>
@@ -6753,9 +6721,9 @@
       <c r="A41" s="7">
         <v>44</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
         <v>43</v>
       </c>
@@ -6773,9 +6741,9 @@
       <c r="A42" s="7">
         <v>45</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="4" t="s">
         <v>46</v>
       </c>
@@ -6793,9 +6761,9 @@
       <c r="A43" s="7">
         <v>46</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
@@ -6813,9 +6781,9 @@
       <c r="A44" s="7">
         <v>47</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="17" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -6835,9 +6803,9 @@
       <c r="A45" s="7">
         <v>48</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
         <v>45</v>
       </c>
@@ -6855,9 +6823,9 @@
       <c r="A46" s="7">
         <v>49</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
@@ -6875,9 +6843,9 @@
       <c r="A47" s="7">
         <v>50</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
@@ -6895,9 +6863,9 @@
       <c r="A48" s="7">
         <v>51</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>46</v>
       </c>
@@ -6915,9 +6883,9 @@
       <c r="A49" s="7">
         <v>52</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="4" t="s">
         <v>44</v>
       </c>
@@ -6933,6 +6901,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:B49"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -6942,15 +6919,6 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B26:B49"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="9" priority="5">
@@ -7047,13 +7015,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -7073,9 +7041,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -7093,9 +7061,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -7113,9 +7081,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -7133,9 +7101,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -7153,9 +7121,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -7175,9 +7143,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -7195,9 +7163,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -7215,11 +7183,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -7237,9 +7205,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -7257,9 +7225,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -7277,9 +7245,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -7297,11 +7265,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -7321,9 +7289,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -7341,9 +7309,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -7361,9 +7329,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -7381,9 +7349,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -7401,9 +7369,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -7421,9 +7389,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -7443,9 +7411,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -7463,9 +7431,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -7483,9 +7451,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -7503,9 +7471,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -7523,9 +7491,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -7543,13 +7511,13 @@
       <c r="A26" s="7">
         <v>29</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -7569,9 +7537,9 @@
       <c r="A27" s="7">
         <v>30</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
@@ -7589,9 +7557,9 @@
       <c r="A28" s="7">
         <v>31</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
@@ -7609,9 +7577,9 @@
       <c r="A29" s="7">
         <v>32</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="10" t="s">
         <v>14</v>
       </c>
@@ -7629,9 +7597,9 @@
       <c r="A30" s="7">
         <v>33</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
@@ -7649,9 +7617,9 @@
       <c r="A31" s="7">
         <v>34</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -7671,9 +7639,9 @@
       <c r="A32" s="7">
         <v>35</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="10" t="s">
         <v>20</v>
       </c>
@@ -7691,9 +7659,9 @@
       <c r="A33" s="7">
         <v>36</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="10" t="s">
         <v>21</v>
       </c>
@@ -7711,11 +7679,11 @@
       <c r="A34" s="7">
         <v>37</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="10" t="s">
         <v>24</v>
       </c>
@@ -7733,9 +7701,9 @@
       <c r="A35" s="7">
         <v>38</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="10" t="s">
         <v>26</v>
       </c>
@@ -7753,9 +7721,9 @@
       <c r="A36" s="7">
         <v>39</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
       <c r="E36" s="10" t="s">
         <v>28</v>
       </c>
@@ -7773,9 +7741,9 @@
       <c r="A37" s="7">
         <v>40</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="10" t="s">
         <v>30</v>
       </c>
@@ -7793,11 +7761,11 @@
       <c r="A38" s="7">
         <v>41</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -7817,9 +7785,9 @@
       <c r="A39" s="7">
         <v>42</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="4" t="s">
         <v>45</v>
       </c>
@@ -7837,9 +7805,9 @@
       <c r="A40" s="7">
         <v>43</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="4" t="s">
         <v>42</v>
       </c>
@@ -7857,9 +7825,9 @@
       <c r="A41" s="7">
         <v>44</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="4" t="s">
         <v>43</v>
       </c>
@@ -7877,9 +7845,9 @@
       <c r="A42" s="7">
         <v>45</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="4" t="s">
         <v>46</v>
       </c>
@@ -7897,9 +7865,9 @@
       <c r="A43" s="7">
         <v>46</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
@@ -7917,9 +7885,9 @@
       <c r="A44" s="7">
         <v>47</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="17" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -7939,9 +7907,9 @@
       <c r="A45" s="7">
         <v>48</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="4" t="s">
         <v>45</v>
       </c>
@@ -7959,9 +7927,9 @@
       <c r="A46" s="7">
         <v>49</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="4" t="s">
         <v>42</v>
       </c>
@@ -7979,9 +7947,9 @@
       <c r="A47" s="7">
         <v>50</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="4" t="s">
         <v>43</v>
       </c>
@@ -7999,9 +7967,9 @@
       <c r="A48" s="7">
         <v>51</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="4" t="s">
         <v>46</v>
       </c>
@@ -8019,9 +7987,9 @@
       <c r="A49" s="7">
         <v>52</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="4" t="s">
         <v>44</v>
       </c>
@@ -8037,6 +8005,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:B49"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -8046,15 +8023,6 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B26:B49"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="4" priority="5">

</xml_diff>

<commit_message>
add foodlist about us test case
</commit_message>
<xml_diff>
--- a/test/IntegrationTest_Index.xlsx
+++ b/test/IntegrationTest_Index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitStar\Panda\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skart\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6225" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Representative" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="86">
   <si>
     <t>design</t>
   </si>
@@ -252,6 +252,51 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>1. click title for each item</t>
+  </si>
+  <si>
+    <t>Go to content page and show the item's information</t>
+  </si>
+  <si>
+    <t>1. click picture</t>
+  </si>
+  <si>
+    <t>1. change page size to mobile screen size, and it will automatically change to mobile design</t>
+  </si>
+  <si>
+    <t>1.click drop down sign
+2.the hidden &lt;div&gt; appear
+3.the drop down arrow "down" change to "up"</t>
+  </si>
+  <si>
+    <t>1.click the "up" arrow 
+2.the &lt;div&gt; disappear and "up" arrow change to "down"</t>
+  </si>
+  <si>
+    <t>1.check the color for different categoaries: meat-red, vegetable-green, dairy product-blue</t>
+  </si>
+  <si>
+    <t>check the hidden &lt;div&gt; tag's content color is the same as their title</t>
+  </si>
+  <si>
+    <t>1. change page size to full of PC horizontality</t>
+  </si>
+  <si>
+    <t>1. change page size to half of PC horizontality</t>
+  </si>
+  <si>
+    <t>1. change page size to small of PC horizontality</t>
+  </si>
+  <si>
+    <t>1. change page size to full of PC verticality</t>
+  </si>
+  <si>
+    <t>1. change page size to half of PC verticality</t>
+  </si>
+  <si>
+    <t>1. change page size to small of PC verticality</t>
   </si>
 </sst>
 </file>
@@ -440,7 +485,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="45">
     <dxf>
       <fill>
         <patternFill>
@@ -459,76 +504,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE8972"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -725,6 +700,90 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1173,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20:J25"/>
     </sheetView>
   </sheetViews>
@@ -2461,21 +2520,21 @@
     <mergeCell ref="D20:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="42" priority="3">
+    <cfRule type="expression" dxfId="44" priority="3">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="4">
+    <cfRule type="expression" dxfId="43" priority="4">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="42" priority="1">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="41" priority="5">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2493,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,7 +2778,7 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2728,38 +2787,50 @@
         <v>1</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3">
+        <v>42870</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="E11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3">
+        <v>42870</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
@@ -2768,18 +2839,14 @@
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -2788,20 +2855,16 @@
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>17</v>
       </c>
@@ -2813,7 +2876,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
@@ -2825,141 +2888,91 @@
       <c r="I14" s="3">
         <v>42870</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>55</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>18</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>19</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>20</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>21</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>22</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -3251,7 +3264,7 @@
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>37</v>
       </c>
@@ -3260,38 +3273,38 @@
         <v>1</v>
       </c>
       <c r="D34" s="17"/>
-      <c r="E34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>38</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
+      <c r="E35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -3300,18 +3313,14 @@
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
@@ -3320,20 +3329,16 @@
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="19"/>
-      <c r="E37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>41</v>
       </c>
@@ -3345,25 +3350,19 @@
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>42</v>
       </c>
@@ -3371,25 +3370,19 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="4" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43</v>
       </c>
@@ -3397,25 +3390,19 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>44</v>
       </c>
@@ -3423,25 +3410,19 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>45</v>
       </c>
@@ -3449,47 +3430,31 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="4" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>46</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="3">
-        <v>42870</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
@@ -3637,22 +3602,55 @@
     <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="40" priority="7">
+    <cfRule type="expression" dxfId="39" priority="16">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="8">
+    <cfRule type="expression" dxfId="38" priority="17">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="38" priority="6">
+  <conditionalFormatting sqref="E2:L9 E44:L49 E15:L33">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="9">
+    <cfRule type="expression" dxfId="36" priority="18">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>$G2="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:L43">
+    <cfRule type="expression" dxfId="34" priority="7">
+      <formula>$K34 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="8">
+      <formula>$G34="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="9">
+      <formula>$G34="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:L13">
+    <cfRule type="expression" dxfId="31" priority="4">
+      <formula>$K10 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="5">
+      <formula>$G10="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="6">
+      <formula>$G10="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:L14">
+    <cfRule type="expression" dxfId="28" priority="1">
+      <formula>$K14 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="2">
+      <formula>$G14="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="3">
+      <formula>$G14="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4741,21 +4739,21 @@
     <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="35" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="33" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6011,32 +6009,32 @@
     <mergeCell ref="C10:C17"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D30 C38:D38 D52:D55 C46:D49 D35">
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>$G30="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>$G30="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:L41 E46:L57 G42:L45">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:F45">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$K42 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>$G42="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$G42="OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6054,8 +6052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6374,7 +6372,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
@@ -6394,7 +6392,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>33</v>
@@ -6414,7 +6412,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>33</v>
@@ -6434,7 +6432,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>33</v>
@@ -6454,7 +6452,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -6474,7 +6472,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>33</v>
@@ -6496,7 +6494,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>33</v>
@@ -6516,7 +6514,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
@@ -6536,7 +6534,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
@@ -6556,7 +6554,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>33</v>
@@ -6576,7 +6574,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>33</v>
@@ -6596,7 +6594,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>33</v>
@@ -6858,7 +6856,7 @@
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
     </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>41</v>
       </c>
@@ -6870,7 +6868,7 @@
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>33</v>
@@ -6882,19 +6880,15 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>42</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -6902,19 +6896,15 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
-      <c r="E40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -6922,19 +6912,15 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>44</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -6942,19 +6928,15 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>45</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -6962,19 +6944,15 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>46</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -6992,7 +6970,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>33</v>
@@ -7012,7 +6990,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>33</v>
@@ -7032,7 +7010,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>33</v>
@@ -7052,7 +7030,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>33</v>
@@ -7072,7 +7050,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>33</v>
@@ -7092,7 +7070,7 @@
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -7126,22 +7104,33 @@
     <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="20" priority="4">
+  <conditionalFormatting sqref="E2:L37 E39:L49 G38:L38">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>$G2="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:F38">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$K38 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$G38="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$G38="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -8230,21 +8219,21 @@
     <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
replace chenge with changne
</commit_message>
<xml_diff>
--- a/test/IntegrationTest_Index.xlsx
+++ b/test/IntegrationTest_Index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skart\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitStar\Panda\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6225" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6225" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Representative" sheetId="9" r:id="rId1"/>
@@ -531,14 +531,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFE8972"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFE8972"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1233,7 +1233,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:J25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,7 +1624,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
@@ -1650,7 +1650,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>33</v>
@@ -1676,7 +1676,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>33</v>
@@ -1702,7 +1702,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>33</v>
@@ -1728,7 +1728,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -1754,7 +1754,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>33</v>
@@ -1782,7 +1782,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>33</v>
@@ -1802,7 +1802,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
@@ -1822,7 +1822,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
@@ -1842,7 +1842,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>33</v>
@@ -1862,7 +1862,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>33</v>
@@ -1882,7 +1882,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>33</v>
@@ -2228,7 +2228,7 @@
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>33</v>
@@ -2254,7 +2254,7 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>33</v>
@@ -2280,7 +2280,7 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>33</v>
@@ -2306,7 +2306,7 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>33</v>
@@ -2332,7 +2332,7 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>33</v>
@@ -2358,7 +2358,7 @@
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
       <c r="E43" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>33</v>
@@ -2386,7 +2386,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>33</v>
@@ -2406,7 +2406,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>33</v>
@@ -2426,7 +2426,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>33</v>
@@ -2446,7 +2446,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>33</v>
@@ -2466,7 +2466,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>33</v>
@@ -2486,7 +2486,7 @@
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -2500,11 +2500,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C49"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="C14:C25"/>
@@ -2512,12 +2513,11 @@
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C49"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="D44:D49"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="44" priority="3">
@@ -3582,6 +3582,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C14:C25"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C10:C13"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D26:D30"/>
@@ -3591,15 +3600,6 @@
     <mergeCell ref="D38:D43"/>
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="39" priority="16">
@@ -3987,7 +3987,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
@@ -4007,7 +4007,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>33</v>
@@ -4027,7 +4027,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>33</v>
@@ -4047,7 +4047,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>33</v>
@@ -4067,7 +4067,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -4087,7 +4087,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>33</v>
@@ -4109,7 +4109,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>33</v>
@@ -4129,7 +4129,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
@@ -4149,7 +4149,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
@@ -4169,7 +4169,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>33</v>
@@ -4189,7 +4189,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>33</v>
@@ -4209,7 +4209,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>33</v>
@@ -4483,7 +4483,7 @@
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>33</v>
@@ -4503,7 +4503,7 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>33</v>
@@ -4523,7 +4523,7 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>33</v>
@@ -4543,7 +4543,7 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>33</v>
@@ -4563,7 +4563,7 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>33</v>
@@ -4583,7 +4583,7 @@
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
       <c r="E43" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>33</v>
@@ -4605,7 +4605,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>33</v>
@@ -4625,7 +4625,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>33</v>
@@ -4645,7 +4645,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>33</v>
@@ -4665,7 +4665,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>33</v>
@@ -4685,7 +4685,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>33</v>
@@ -4705,7 +4705,7 @@
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -4719,6 +4719,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C14:C25"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C10:C13"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D26:D30"/>
@@ -4728,15 +4737,6 @@
     <mergeCell ref="D38:D43"/>
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="25" priority="5">
@@ -5173,7 +5173,7 @@
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -5193,7 +5193,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>33</v>
@@ -5213,7 +5213,7 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>33</v>
@@ -5233,7 +5233,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
@@ -5253,7 +5253,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
@@ -5273,7 +5273,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>33</v>
@@ -5295,7 +5295,7 @@
         <v>34</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>33</v>
@@ -5315,7 +5315,7 @@
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>33</v>
@@ -5335,7 +5335,7 @@
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>33</v>
@@ -5355,7 +5355,7 @@
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>33</v>
@@ -5375,7 +5375,7 @@
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>33</v>
@@ -5395,7 +5395,7 @@
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
       <c r="E29" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>33</v>
@@ -5751,7 +5751,7 @@
         <v>32</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>33</v>
@@ -5771,7 +5771,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>33</v>
@@ -5791,7 +5791,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>33</v>
@@ -5811,7 +5811,7 @@
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -5831,7 +5831,7 @@
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
       <c r="E50" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>33</v>
@@ -5851,7 +5851,7 @@
       <c r="C51" s="18"/>
       <c r="D51" s="19"/>
       <c r="E51" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>33</v>
@@ -5873,7 +5873,7 @@
         <v>34</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>33</v>
@@ -5893,7 +5893,7 @@
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
       <c r="E53" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>33</v>
@@ -5913,7 +5913,7 @@
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
       <c r="E54" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>33</v>
@@ -5933,7 +5933,7 @@
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>33</v>
@@ -5953,7 +5953,7 @@
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
       <c r="E56" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>33</v>
@@ -5973,7 +5973,7 @@
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
       <c r="E57" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>33</v>
@@ -5987,6 +5987,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2:B29"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C18:C29"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C10:C17"/>
     <mergeCell ref="B30:B57"/>
     <mergeCell ref="C30:C37"/>
     <mergeCell ref="D30:D34"/>
@@ -5997,16 +6007,6 @@
     <mergeCell ref="D52:D57"/>
     <mergeCell ref="C38:C45"/>
     <mergeCell ref="D42:D45"/>
-    <mergeCell ref="B2:B29"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C18:C29"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C10:C17"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D30 C38:D38 D52:D55 C46:D49 D35">
     <cfRule type="expression" dxfId="20" priority="5">
@@ -6052,7 +6052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -7084,6 +7084,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C14:C25"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C10:C13"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D26:D30"/>
@@ -7093,15 +7102,6 @@
     <mergeCell ref="D38:D43"/>
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
     <cfRule type="expression" dxfId="12" priority="8">
@@ -7123,13 +7123,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:F38">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$K38 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$G38="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$G38="OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7147,8 +7147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7467,7 +7467,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
@@ -7487,7 +7487,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>33</v>
@@ -7507,7 +7507,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>33</v>
@@ -7527,7 +7527,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>33</v>
@@ -7547,7 +7547,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -7567,7 +7567,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>33</v>
@@ -7589,7 +7589,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>33</v>
@@ -7609,7 +7609,7 @@
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
@@ -7629,7 +7629,7 @@
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
@@ -7649,7 +7649,7 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>33</v>
@@ -7669,7 +7669,7 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>33</v>
@@ -7689,7 +7689,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>33</v>
@@ -7963,7 +7963,7 @@
         <v>32</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>33</v>
@@ -7983,7 +7983,7 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>33</v>
@@ -8003,7 +8003,7 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>33</v>
@@ -8023,7 +8023,7 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>33</v>
@@ -8043,7 +8043,7 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>33</v>
@@ -8063,7 +8063,7 @@
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
       <c r="E43" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>33</v>
@@ -8085,7 +8085,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>33</v>
@@ -8105,7 +8105,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>33</v>
@@ -8125,7 +8125,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>33</v>
@@ -8145,7 +8145,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>33</v>
@@ -8165,7 +8165,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>33</v>
@@ -8185,7 +8185,7 @@
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="4" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -8199,6 +8199,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C14:C25"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C10:C13"/>
     <mergeCell ref="B26:B49"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D26:D30"/>
@@ -8208,32 +8217,23 @@
     <mergeCell ref="D38:D43"/>
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C14:C25"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C10:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D44:D47 C38:D41 D31">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$G26="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$G26="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:L49">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
modify base.css to fix the navi bar on foodlist, add sql
</commit_message>
<xml_diff>
--- a/test/IntegrationTest_Index.xlsx
+++ b/test/IntegrationTest_Index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haruna Doranecoco\comp2910\Panda\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakit\Desktop\web\Panda\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6230" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9450" windowHeight="6230" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Representative" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="101">
   <si>
     <t>design</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Input fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In category panel, search button should be right place </t>
+  </si>
+  <si>
+    <t>category panel looks different from firefox, and content page</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -579,10 +585,25 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -591,18 +612,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -610,7 +619,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="69">
     <dxf>
       <fill>
         <patternFill>
@@ -755,6 +764,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFE8972"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1571,13 +1601,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1603,9 +1633,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1629,9 +1659,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1655,9 +1685,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1681,9 +1711,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1707,9 +1737,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1735,9 +1765,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1761,9 +1791,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1787,11 +1817,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
@@ -1815,9 +1845,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1841,9 +1871,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1867,9 +1897,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1893,11 +1923,11 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1923,9 +1953,9 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -1949,9 +1979,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1977,9 +2007,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2003,9 +2033,9 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -2031,9 +2061,9 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -2059,9 +2089,9 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="39" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -2083,9 +2113,9 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -2105,9 +2135,9 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -2133,9 +2163,9 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -2159,9 +2189,9 @@
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -2187,9 +2217,9 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -2215,13 +2245,13 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="40" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -2247,9 +2277,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
@@ -2273,9 +2303,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
       <c r="E28" s="4" t="s">
         <v>13</v>
       </c>
@@ -2299,9 +2329,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="4" t="s">
         <v>14</v>
       </c>
@@ -2325,9 +2355,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
@@ -2351,9 +2381,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -2379,9 +2409,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="4" t="s">
         <v>20</v>
       </c>
@@ -2405,9 +2435,9 @@
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
       <c r="E33" s="4" t="s">
         <v>21</v>
       </c>
@@ -2431,11 +2461,11 @@
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38" t="s">
+      <c r="B34" s="40"/>
+      <c r="C34" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="38"/>
+      <c r="D34" s="40"/>
       <c r="E34" s="4" t="s">
         <v>24</v>
       </c>
@@ -2459,9 +2489,9 @@
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
       <c r="E35" s="4" t="s">
         <v>26</v>
       </c>
@@ -2485,9 +2515,9 @@
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
       <c r="E36" s="4" t="s">
         <v>28</v>
       </c>
@@ -2511,9 +2541,9 @@
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="4" t="s">
         <v>30</v>
       </c>
@@ -2537,17 +2567,17 @@
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38" t="s">
+      <c r="B38" s="40"/>
+      <c r="C38" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="41" t="s">
         <v>33</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -2571,11 +2601,11 @@
     </row>
     <row r="39" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
       <c r="G39" s="2" t="s">
         <v>72</v>
       </c>
@@ -2595,8 +2625,8 @@
       <c r="A40" s="7">
         <v>38</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="18" t="s">
         <v>34</v>
       </c>
@@ -2627,11 +2657,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C14:C25"/>
     <mergeCell ref="C10:C13"/>
@@ -2640,21 +2671,20 @@
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:L38 E40:L40 G39:L39">
-    <cfRule type="expression" dxfId="65" priority="4">
+    <cfRule type="expression" dxfId="68" priority="4">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="8">
+    <cfRule type="expression" dxfId="67" priority="8">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="9">
+    <cfRule type="expression" dxfId="66" priority="9">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2670,13 +2700,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2737,13 +2767,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -2763,9 +2793,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -2783,9 +2813,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -2803,9 +2833,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -2823,9 +2853,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -2841,9 +2871,9 @@
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -2861,9 +2891,9 @@
     </row>
     <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -2879,9 +2909,9 @@
     </row>
     <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -2899,11 +2929,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -2921,9 +2951,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2941,9 +2971,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -2961,9 +2991,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -2981,11 +3011,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -3013,9 +3043,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -3039,9 +3069,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -3065,9 +3095,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -3091,9 +3121,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -3119,9 +3149,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -3147,9 +3177,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="39" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -3177,9 +3207,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -3203,9 +3233,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -3229,9 +3259,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="21" t="s">
         <v>43</v>
       </c>
@@ -3249,9 +3279,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -3277,9 +3307,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -3305,13 +3335,13 @@
       <c r="A26" s="7">
         <v>29</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="40" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -3331,9 +3361,9 @@
       <c r="A27" s="7">
         <v>30</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="10" t="s">
         <v>11</v>
       </c>
@@ -3351,9 +3381,9 @@
       <c r="A28" s="7">
         <v>31</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
       <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
@@ -3371,9 +3401,9 @@
       <c r="A29" s="7">
         <v>32</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="10" t="s">
         <v>14</v>
       </c>
@@ -3391,9 +3421,9 @@
       <c r="A30" s="7">
         <v>33</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
@@ -3411,9 +3441,9 @@
       <c r="A31" s="7">
         <v>34</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -3433,9 +3463,9 @@
       <c r="A32" s="7">
         <v>35</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="10" t="s">
         <v>20</v>
       </c>
@@ -3453,9 +3483,9 @@
       <c r="A33" s="7">
         <v>36</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
       <c r="E33" s="10" t="s">
         <v>21</v>
       </c>
@@ -3473,9 +3503,9 @@
       <c r="A34" s="7">
         <v>34</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38" t="s">
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40" t="s">
         <v>79</v>
       </c>
       <c r="E34" s="19" t="s">
@@ -3501,9 +3531,9 @@
       <c r="A35" s="7">
         <v>35</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
       <c r="E35" s="19" t="s">
         <v>82</v>
       </c>
@@ -3527,11 +3557,11 @@
       <c r="A36" s="7">
         <v>37</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38" t="s">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="38"/>
+      <c r="D36" s="40"/>
       <c r="E36" s="13" t="s">
         <v>24</v>
       </c>
@@ -3549,9 +3579,9 @@
       <c r="A37" s="7">
         <v>38</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="13" t="s">
         <v>26</v>
       </c>
@@ -3569,9 +3599,9 @@
       <c r="A38" s="7">
         <v>39</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="13" t="s">
         <v>28</v>
       </c>
@@ -3589,9 +3619,9 @@
       <c r="A39" s="7">
         <v>40</v>
       </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="13" t="s">
         <v>30</v>
       </c>
@@ -3609,17 +3639,17 @@
       <c r="A40" s="7">
         <v>41</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38" t="s">
+      <c r="B40" s="40"/>
+      <c r="C40" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F40" s="42" t="s">
+      <c r="F40" s="43" t="s">
         <v>33</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -3642,55 +3672,47 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="7">
-        <v>42</v>
-      </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="2" t="s">
+      <c r="A41" s="28"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="24" t="s">
         <v>85</v>
       </c>
       <c r="I41" s="3">
         <v>42871</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="24"/>
     </row>
     <row r="42" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
-        <v>43</v>
-      </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" s="42" t="s">
-        <v>33</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
       <c r="G42" s="2" t="s">
         <v>72</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="I42" s="3">
         <v>42871</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="K42" s="3">
         <v>42871</v>
@@ -3699,47 +3721,66 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
-        <v>44</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
+        <v>43</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>33</v>
+      </c>
       <c r="G43" s="2" t="s">
         <v>72</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I43" s="3">
         <v>42871</v>
       </c>
       <c r="J43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K43" s="3">
+        <v>42871</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="7">
+        <v>44</v>
+      </c>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I44" s="3">
+        <v>42871</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B26:B43"/>
-    <mergeCell ref="C26:C35"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="C40:C43"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -3748,130 +3789,134 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B26:B44"/>
+    <mergeCell ref="C26:C35"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:L6 G7:L9 F40:G40 I40:L40 E34:L39 E10:L30 K41:L43">
-    <cfRule type="expression" dxfId="62" priority="48">
+  <conditionalFormatting sqref="E2:L6 G7:L9 F40:G40 I40:L40 E34:L39 E10:L30 E43:F43 K41:L44 F41">
+    <cfRule type="expression" dxfId="65" priority="54">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51">
+    <cfRule type="expression" dxfId="64" priority="57">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52">
+    <cfRule type="expression" dxfId="63" priority="58">
       <formula>$G2="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="59" priority="37">
+  <conditionalFormatting sqref="E40:E41">
+    <cfRule type="expression" dxfId="62" priority="43">
       <formula>$K40 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="38">
+    <cfRule type="expression" dxfId="61" priority="44">
       <formula>$G40="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="39">
+    <cfRule type="expression" dxfId="60" priority="45">
       <formula>$G40="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F9">
-    <cfRule type="expression" dxfId="56" priority="31">
+    <cfRule type="expression" dxfId="59" priority="37">
       <formula>$K7 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="32">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>$G7="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="33">
+    <cfRule type="expression" dxfId="57" priority="39">
       <formula>$G7="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:L33">
-    <cfRule type="expression" dxfId="53" priority="28">
+    <cfRule type="expression" dxfId="56" priority="34">
       <formula>$K31 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="29">
+    <cfRule type="expression" dxfId="55" priority="35">
       <formula>$G31="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="30">
+    <cfRule type="expression" dxfId="54" priority="36">
       <formula>$G31="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="50" priority="25">
+    <cfRule type="expression" dxfId="53" priority="31">
       <formula>$K40 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="26">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>$G40="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="27">
+    <cfRule type="expression" dxfId="51" priority="33">
       <formula>$G40="OK"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G42:J42">
+    <cfRule type="expression" dxfId="50" priority="22">
+      <formula>$K42 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="23">
+      <formula>$G42="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="24">
+      <formula>$G42="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43 I43:J43">
+    <cfRule type="expression" dxfId="47" priority="19">
+      <formula>$K43 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="20">
+      <formula>$G43="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="21">
+      <formula>$G43="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="expression" dxfId="44" priority="16">
+      <formula>$K43 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="17">
+      <formula>$G43="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="18">
+      <formula>$G43="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44:J44">
+    <cfRule type="expression" dxfId="41" priority="13">
+      <formula>$K44 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="14">
+      <formula>$G44="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="15">
+      <formula>$G44="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G41:J41">
-    <cfRule type="expression" dxfId="47" priority="16">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>$K41 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="17">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>$G41="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="18">
+    <cfRule type="expression" dxfId="36" priority="3">
       <formula>$G41="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42 I42:J42">
-    <cfRule type="expression" dxfId="44" priority="13">
-      <formula>$K42 &lt;&gt; ""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="14">
-      <formula>$G42="NG"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="15">
-      <formula>$G42="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="41" priority="10">
-      <formula>$K42 &lt;&gt; ""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="11">
-      <formula>$G42="NG"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="12">
-      <formula>$G42="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43:J43">
-    <cfRule type="expression" dxfId="38" priority="7">
-      <formula>$K43 &lt;&gt; ""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="8">
-      <formula>$G43="NG"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="9">
-      <formula>$G43="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="35" priority="4">
-      <formula>$K42 &lt;&gt; ""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="5">
-      <formula>$G42="NG"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="6">
-      <formula>$G42="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="32" priority="1">
-      <formula>$K42 &lt;&gt; ""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="2">
-      <formula>$G42="NG"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="3">
-      <formula>$G42="OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G44">
       <formula1>"OK, NG"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3884,11 +3929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G39" sqref="G39:J39"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3949,13 +3994,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -3975,9 +4020,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -3995,9 +4040,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -4015,9 +4060,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -4035,9 +4080,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -4055,9 +4100,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -4077,9 +4122,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -4097,9 +4142,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -4117,11 +4162,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -4139,9 +4184,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -4159,9 +4204,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -4179,9 +4224,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -4199,11 +4244,11 @@
       <c r="A14" s="7">
         <v>17</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -4229,9 +4274,9 @@
       <c r="A15" s="7">
         <v>18</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
@@ -4255,9 +4300,9 @@
       <c r="A16" s="7">
         <v>19</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
@@ -4281,9 +4326,9 @@
       <c r="A17" s="7">
         <v>20</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
@@ -4307,9 +4352,9 @@
       <c r="A18" s="7">
         <v>21</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
@@ -4333,9 +4378,9 @@
       <c r="A19" s="7">
         <v>22</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="4" t="s">
         <v>44</v>
       </c>
@@ -4359,9 +4404,9 @@
       <c r="A20" s="7">
         <v>23</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="39" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -4387,9 +4432,9 @@
       <c r="A21" s="7">
         <v>24</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
@@ -4413,9 +4458,9 @@
       <c r="A22" s="7">
         <v>25</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -4439,9 +4484,9 @@
       <c r="A23" s="7">
         <v>26</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
@@ -4465,9 +4510,9 @@
       <c r="A24" s="7">
         <v>27</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
@@ -4491,9 +4536,9 @@
       <c r="A25" s="7">
         <v>28</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
@@ -4517,13 +4562,13 @@
       <c r="A26" s="28">
         <v>29</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="29" t="s">
@@ -4543,9 +4588,9 @@
       <c r="A27" s="28">
         <v>30</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="29" t="s">
         <v>11</v>
       </c>
@@ -4563,9 +4608,9 @@
       <c r="A28" s="28">
         <v>31</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="29" t="s">
         <v>13</v>
       </c>
@@ -4583,9 +4628,9 @@
       <c r="A29" s="28">
         <v>32</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="29" t="s">
         <v>14</v>
       </c>
@@ -4603,9 +4648,9 @@
       <c r="A30" s="28">
         <v>33</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="40"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="29" t="s">
         <v>17</v>
       </c>
@@ -4623,9 +4668,9 @@
       <c r="A31" s="28">
         <v>34</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="39" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="29" t="s">
@@ -4645,9 +4690,9 @@
       <c r="A32" s="28">
         <v>35</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="29" t="s">
         <v>20</v>
       </c>
@@ -4665,9 +4710,9 @@
       <c r="A33" s="28">
         <v>36</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="29" t="s">
         <v>21</v>
       </c>
@@ -4685,11 +4730,11 @@
       <c r="A34" s="28">
         <v>37</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="39" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="32" t="s">
         <v>24</v>
       </c>
@@ -4707,9 +4752,9 @@
       <c r="A35" s="28">
         <v>38</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="32" t="s">
         <v>26</v>
       </c>
@@ -4727,9 +4772,9 @@
       <c r="A36" s="28">
         <v>39</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="32" t="s">
         <v>28</v>
       </c>
@@ -4747,9 +4792,9 @@
       <c r="A37" s="28">
         <v>40</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="40"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="32" t="s">
         <v>30</v>
       </c>
@@ -4763,15 +4808,15 @@
       <c r="K37" s="33"/>
       <c r="L37" s="33"/>
     </row>
-    <row r="38" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="28">
         <v>41</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="39" t="s">
+      <c r="B38" s="38"/>
+      <c r="C38" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="36" t="s">
         <v>32</v>
       </c>
       <c r="E38" s="25" t="s">
@@ -4781,25 +4826,25 @@
         <v>33</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H38" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>99</v>
+      </c>
       <c r="I38" s="3">
         <v>42871</v>
       </c>
       <c r="J38" s="24" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
     </row>
-    <row r="39" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="28">
-        <v>42</v>
-      </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="34" t="s">
+    <row r="39" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="28"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="35" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="25" t="s">
@@ -4809,20 +4854,29 @@
         <v>33</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H39" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>99</v>
+      </c>
       <c r="I39" s="3">
         <v>42871</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B26:B39"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="C38:C39"/>
     <mergeCell ref="B2:B25"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -4832,23 +4886,27 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B26:B39"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="C38:C39"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:L37 F38:L39">
-    <cfRule type="expression" dxfId="29" priority="19">
+  <conditionalFormatting sqref="K39:L39 E2:L38">
+    <cfRule type="expression" dxfId="35" priority="28">
       <formula>$K2 &lt;&gt; ""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="22">
+    <cfRule type="expression" dxfId="34" priority="31">
       <formula>$G2="NG"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="23">
+    <cfRule type="expression" dxfId="33" priority="32">
       <formula>$G2="OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39:G39">
+    <cfRule type="expression" dxfId="29" priority="7">
+      <formula>$K39 &lt;&gt; ""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="8">
+      <formula>$G39="NG"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="9">
+      <formula>$G39="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
@@ -4862,15 +4920,15 @@
       <formula>$G39="OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
+  <conditionalFormatting sqref="H39:J39">
     <cfRule type="expression" dxfId="23" priority="1">
-      <formula>$K38 &lt;&gt; ""</formula>
+      <formula>$K39 &lt;&gt; ""</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="2">
-      <formula>$G38="NG"</formula>
+      <formula>$G39="NG"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="3">
-      <formula>$G38="OK"</formula>
+      <formula>$G39="OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4949,13 +5007,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -4975,9 +5033,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -4995,9 +5053,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -5015,9 +5073,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -5035,9 +5093,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -5055,9 +5113,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -5077,9 +5135,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -5097,9 +5155,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -5117,11 +5175,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -5139,9 +5197,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -5159,9 +5217,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -5179,9 +5237,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -5199,9 +5257,9 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="39" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="37" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -5221,9 +5279,9 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="15" t="s">
         <v>67</v>
       </c>
@@ -5241,9 +5299,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="15" t="s">
         <v>68</v>
       </c>
@@ -5261,9 +5319,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="15" t="s">
         <v>69</v>
       </c>
@@ -5281,11 +5339,11 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -5305,9 +5363,9 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="4" t="s">
         <v>45</v>
       </c>
@@ -5325,9 +5383,9 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
@@ -5345,9 +5403,9 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4" t="s">
         <v>43</v>
       </c>
@@ -5365,9 +5423,9 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="4" t="s">
         <v>46</v>
       </c>
@@ -5385,9 +5443,9 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="40"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="4" t="s">
         <v>44</v>
       </c>
@@ -5405,9 +5463,9 @@
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="39" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -5427,9 +5485,9 @@
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
@@ -5447,9 +5505,9 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="4" t="s">
         <v>42</v>
       </c>
@@ -5467,9 +5525,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="4" t="s">
         <v>43</v>
       </c>
@@ -5487,9 +5545,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="4" t="s">
         <v>46</v>
       </c>
@@ -5507,9 +5565,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="4" t="s">
         <v>44</v>
       </c>
@@ -5527,13 +5585,13 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="10" t="s">
@@ -5553,9 +5611,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="10" t="s">
         <v>11</v>
       </c>
@@ -5573,9 +5631,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="10" t="s">
         <v>13</v>
       </c>
@@ -5593,9 +5651,9 @@
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
       <c r="E33" s="10" t="s">
         <v>14</v>
       </c>
@@ -5613,9 +5671,9 @@
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="40"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="39"/>
       <c r="E34" s="10" t="s">
         <v>17</v>
       </c>
@@ -5633,9 +5691,9 @@
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="39" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="10" t="s">
@@ -5655,9 +5713,9 @@
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="10" t="s">
         <v>20</v>
       </c>
@@ -5675,9 +5733,9 @@
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="10" t="s">
         <v>21</v>
       </c>
@@ -5695,11 +5753,11 @@
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="39" t="s">
+      <c r="B38" s="38"/>
+      <c r="C38" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="39"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="10" t="s">
         <v>24</v>
       </c>
@@ -5717,9 +5775,9 @@
       <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="10" t="s">
         <v>26</v>
       </c>
@@ -5737,9 +5795,9 @@
       <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="10" t="s">
         <v>28</v>
       </c>
@@ -5757,9 +5815,9 @@
       <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="40"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="39"/>
       <c r="E41" s="10" t="s">
         <v>30</v>
       </c>
@@ -5777,9 +5835,9 @@
       <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="39" t="s">
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="37" t="s">
         <v>62</v>
       </c>
       <c r="E42" s="13" t="s">
@@ -5799,9 +5857,9 @@
       <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
       <c r="E43" s="13" t="s">
         <v>67</v>
       </c>
@@ -5819,9 +5877,9 @@
       <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="13" t="s">
         <v>68</v>
       </c>
@@ -5839,9 +5897,9 @@
       <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="41"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="13" t="s">
         <v>69</v>
       </c>
@@ -5859,11 +5917,11 @@
       <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="39" t="s">
+      <c r="B46" s="38"/>
+      <c r="C46" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="34" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -5883,9 +5941,9 @@
       <c r="A47" s="7">
         <v>51</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="39" t="s">
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E47" s="4" t="s">
@@ -5905,9 +5963,9 @@
       <c r="A48" s="7">
         <v>52</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
@@ -5925,9 +5983,9 @@
       <c r="A49" s="7">
         <v>53</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
       <c r="E49" s="4" t="s">
         <v>42</v>
       </c>
@@ -5945,9 +6003,9 @@
       <c r="A50" s="7">
         <v>54</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
       <c r="E50" s="4" t="s">
         <v>43</v>
       </c>
@@ -5965,9 +6023,9 @@
       <c r="A51" s="7">
         <v>55</v>
       </c>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
       <c r="E51" s="4" t="s">
         <v>46</v>
       </c>
@@ -5985,9 +6043,9 @@
       <c r="A52" s="7">
         <v>56</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
       <c r="E52" s="4" t="s">
         <v>44</v>
       </c>
@@ -6003,6 +6061,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B30:B52"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C46:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="C38:C45"/>
+    <mergeCell ref="D42:D45"/>
     <mergeCell ref="B2:B29"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -6013,15 +6080,6 @@
     <mergeCell ref="D24:D29"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="C10:C17"/>
-    <mergeCell ref="B30:B52"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C46:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="C38:C45"/>
-    <mergeCell ref="D42:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D30 C38:D38 D47:D50 D35 C46:D46">
     <cfRule type="expression" dxfId="20" priority="5">
@@ -6129,13 +6187,13 @@
       <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -6155,9 +6213,9 @@
       <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="29" t="s">
         <v>11</v>
       </c>
@@ -6175,9 +6233,9 @@
       <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="29" t="s">
         <v>13</v>
       </c>
@@ -6195,9 +6253,9 @@
       <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="29" t="s">
         <v>14</v>
       </c>
@@ -6215,9 +6273,9 @@
       <c r="A6" s="28">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="29" t="s">
         <v>17</v>
       </c>
@@ -6235,9 +6293,9 @@
       <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="29" t="s">
@@ -6257,9 +6315,9 @@
       <c r="A8" s="28">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="29" t="s">
         <v>20</v>
       </c>
@@ -6277,9 +6335,9 @@
       <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="29" t="s">
         <v>21</v>
       </c>
@@ -6297,11 +6355,11 @@
       <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="32" t="s">
         <v>24</v>
       </c>
@@ -6319,9 +6377,9 @@
       <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="32" t="s">
         <v>26</v>
       </c>
@@ -6339,9 +6397,9 @@
       <c r="A12" s="28">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="32" t="s">
         <v>28</v>
       </c>
@@ -6359,9 +6417,9 @@
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="32" t="s">
         <v>30</v>
       </c>
@@ -6379,11 +6437,11 @@
       <c r="A14" s="28">
         <v>15</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -6403,9 +6461,9 @@
       <c r="A15" s="28">
         <v>16</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="25" t="s">
         <v>87</v>
       </c>
@@ -6423,9 +6481,9 @@
       <c r="A16" s="28">
         <v>17</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="25" t="s">
         <v>88</v>
       </c>
@@ -6443,9 +6501,9 @@
       <c r="A17" s="28">
         <v>18</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="25" t="s">
         <v>89</v>
       </c>
@@ -6463,9 +6521,9 @@
       <c r="A18" s="28">
         <v>19</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="25" t="s">
         <v>90</v>
       </c>
@@ -6483,9 +6541,9 @@
       <c r="A19" s="28">
         <v>20</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="25" t="s">
         <v>91</v>
       </c>
@@ -6503,9 +6561,9 @@
       <c r="A20" s="28">
         <v>21</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="39" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -6525,9 +6583,9 @@
       <c r="A21" s="28">
         <v>22</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="25" t="s">
         <v>87</v>
       </c>
@@ -6545,9 +6603,9 @@
       <c r="A22" s="28">
         <v>23</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="25" t="s">
         <v>88</v>
       </c>
@@ -6565,9 +6623,9 @@
       <c r="A23" s="28">
         <v>24</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="25" t="s">
         <v>89</v>
       </c>
@@ -6585,9 +6643,9 @@
       <c r="A24" s="28">
         <v>25</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="25" t="s">
         <v>90</v>
       </c>
@@ -6605,9 +6663,9 @@
       <c r="A25" s="28">
         <v>26</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="25" t="s">
         <v>91</v>
       </c>
@@ -6625,13 +6683,13 @@
       <c r="A26" s="28">
         <v>27</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="29" t="s">
@@ -6651,9 +6709,9 @@
       <c r="A27" s="28">
         <v>28</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="29" t="s">
         <v>11</v>
       </c>
@@ -6671,9 +6729,9 @@
       <c r="A28" s="28">
         <v>29</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="29" t="s">
         <v>13</v>
       </c>
@@ -6691,9 +6749,9 @@
       <c r="A29" s="28">
         <v>30</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="29" t="s">
         <v>14</v>
       </c>
@@ -6711,9 +6769,9 @@
       <c r="A30" s="28">
         <v>31</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="40"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="29" t="s">
         <v>17</v>
       </c>
@@ -6731,9 +6789,9 @@
       <c r="A31" s="28">
         <v>32</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="39" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="29" t="s">
@@ -6753,9 +6811,9 @@
       <c r="A32" s="28">
         <v>33</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="29" t="s">
         <v>20</v>
       </c>
@@ -6773,9 +6831,9 @@
       <c r="A33" s="28">
         <v>34</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="29" t="s">
         <v>21</v>
       </c>
@@ -6793,11 +6851,11 @@
       <c r="A34" s="28">
         <v>35</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="39" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="29" t="s">
         <v>24</v>
       </c>
@@ -6815,9 +6873,9 @@
       <c r="A35" s="28">
         <v>36</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="29" t="s">
         <v>26</v>
       </c>
@@ -6835,9 +6893,9 @@
       <c r="A36" s="28">
         <v>37</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="29" t="s">
         <v>28</v>
       </c>
@@ -6855,9 +6913,9 @@
       <c r="A37" s="28">
         <v>38</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="40"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="29" t="s">
         <v>30</v>
       </c>
@@ -6875,9 +6933,9 @@
       <c r="A38" s="28">
         <v>39</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="25" t="s">
         <v>86</v>
       </c>
@@ -6895,9 +6953,9 @@
       <c r="A39" s="28">
         <v>40</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="25" t="s">
         <v>87</v>
       </c>
@@ -6915,9 +6973,9 @@
       <c r="A40" s="28">
         <v>41</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="25" t="s">
         <v>88</v>
       </c>
@@ -6935,9 +6993,9 @@
       <c r="A41" s="28">
         <v>42</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
       <c r="E41" s="25" t="s">
         <v>89</v>
       </c>
@@ -6955,9 +7013,9 @@
       <c r="A42" s="28">
         <v>43</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="40"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="25" t="s">
         <v>90</v>
       </c>
@@ -6975,9 +7033,9 @@
       <c r="A43" s="28">
         <v>44</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="39" t="s">
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E43" s="25" t="s">
@@ -6997,9 +7055,9 @@
       <c r="A44" s="28">
         <v>45</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="25" t="s">
         <v>87</v>
       </c>
@@ -7017,9 +7075,9 @@
       <c r="A45" s="28">
         <v>46</v>
       </c>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
       <c r="E45" s="25" t="s">
         <v>88</v>
       </c>
@@ -7037,9 +7095,9 @@
       <c r="A46" s="28">
         <v>47</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
       <c r="E46" s="25" t="s">
         <v>89</v>
       </c>
@@ -7057,9 +7115,9 @@
       <c r="A47" s="28">
         <v>48</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
       <c r="E47" s="25" t="s">
         <v>90</v>
       </c>
@@ -7077,9 +7135,9 @@
       <c r="A48" s="28">
         <v>49</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
       <c r="E48" s="25" t="s">
         <v>91</v>
       </c>
@@ -7095,6 +7153,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="C34:C37"/>
     <mergeCell ref="B26:B48"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D26:D30"/>
@@ -7111,8 +7171,6 @@
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="C38:C48"/>
     <mergeCell ref="D38:D42"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:D26 C34:D34 D43:D46 D31 C38:D40">
     <cfRule type="expression" dxfId="12" priority="5">
@@ -7147,7 +7205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B29"/>
     </sheetView>
   </sheetViews>
@@ -7209,13 +7267,13 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -7235,9 +7293,9 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
@@ -7255,9 +7313,9 @@
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
@@ -7275,9 +7333,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
@@ -7295,9 +7353,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
@@ -7315,9 +7373,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="39" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -7337,9 +7395,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
@@ -7357,9 +7415,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
@@ -7377,11 +7435,11 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="13" t="s">
         <v>24</v>
       </c>
@@ -7399,9 +7457,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
@@ -7419,9 +7477,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -7439,9 +7497,9 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="13" t="s">
         <v>30</v>
       </c>
@@ -7459,11 +7517,11 @@
       <c r="A14" s="28">
         <v>13</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -7483,9 +7541,9 @@
       <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="15" t="s">
         <v>93</v>
       </c>
@@ -7503,9 +7561,9 @@
       <c r="A16" s="28">
         <v>15</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="15" t="s">
         <v>94</v>
       </c>
@@ -7523,9 +7581,9 @@
       <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="15" t="s">
         <v>95</v>
       </c>
@@ -7543,11 +7601,11 @@
       <c r="A18" s="28">
         <v>17</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -7567,9 +7625,9 @@
       <c r="A19" s="28">
         <v>18</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="4" t="s">
         <v>45</v>
       </c>
@@ -7587,9 +7645,9 @@
       <c r="A20" s="28">
         <v>19</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
@@ -7607,9 +7665,9 @@
       <c r="A21" s="28">
         <v>20</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4" t="s">
         <v>43</v>
       </c>
@@ -7627,9 +7685,9 @@
       <c r="A22" s="28">
         <v>21</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="4" t="s">
         <v>46</v>
       </c>
@@ -7647,9 +7705,9 @@
       <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="40"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="4" t="s">
         <v>44</v>
       </c>
@@ -7667,9 +7725,9 @@
       <c r="A24" s="28">
         <v>23</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="39" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -7689,9 +7747,9 @@
       <c r="A25" s="28">
         <v>24</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
@@ -7709,9 +7767,9 @@
       <c r="A26" s="28">
         <v>25</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="4" t="s">
         <v>42</v>
       </c>
@@ -7729,9 +7787,9 @@
       <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="4" t="s">
         <v>43</v>
       </c>
@@ -7749,9 +7807,9 @@
       <c r="A28" s="28">
         <v>27</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="4" t="s">
         <v>46</v>
       </c>
@@ -7769,9 +7827,9 @@
       <c r="A29" s="28">
         <v>28</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="4" t="s">
         <v>44</v>
       </c>
@@ -7789,13 +7847,13 @@
       <c r="A30" s="28">
         <v>29</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="37" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="10" t="s">
@@ -7815,9 +7873,9 @@
       <c r="A31" s="28">
         <v>30</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="10" t="s">
         <v>11</v>
       </c>
@@ -7835,9 +7893,9 @@
       <c r="A32" s="28">
         <v>31</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="10" t="s">
         <v>13</v>
       </c>
@@ -7855,9 +7913,9 @@
       <c r="A33" s="28">
         <v>32</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
       <c r="E33" s="10" t="s">
         <v>14</v>
       </c>
@@ -7875,9 +7933,9 @@
       <c r="A34" s="28">
         <v>33</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="40"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="39"/>
       <c r="E34" s="10" t="s">
         <v>17</v>
       </c>
@@ -7895,9 +7953,9 @@
       <c r="A35" s="28">
         <v>34</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="39" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="37" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="10" t="s">
@@ -7917,9 +7975,9 @@
       <c r="A36" s="28">
         <v>35</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="10" t="s">
         <v>20</v>
       </c>
@@ -7937,9 +7995,9 @@
       <c r="A37" s="28">
         <v>36</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
       <c r="E37" s="10" t="s">
         <v>21</v>
       </c>
@@ -7957,11 +8015,11 @@
       <c r="A38" s="28">
         <v>37</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="39" t="s">
+      <c r="B38" s="38"/>
+      <c r="C38" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="39"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="10" t="s">
         <v>24</v>
       </c>
@@ -7979,9 +8037,9 @@
       <c r="A39" s="28">
         <v>38</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="10" t="s">
         <v>26</v>
       </c>
@@ -7999,9 +8057,9 @@
       <c r="A40" s="28">
         <v>39</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="10" t="s">
         <v>28</v>
       </c>
@@ -8019,9 +8077,9 @@
       <c r="A41" s="28">
         <v>40</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
       <c r="E41" s="10" t="s">
         <v>30</v>
       </c>
@@ -8039,11 +8097,11 @@
       <c r="A42" s="28">
         <v>41</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41" t="s">
+      <c r="B42" s="38"/>
+      <c r="C42" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="37" t="s">
         <v>98</v>
       </c>
       <c r="E42" s="32" t="s">
@@ -8063,9 +8121,9 @@
       <c r="A43" s="28">
         <v>42</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
       <c r="E43" s="32" t="s">
         <v>93</v>
       </c>
@@ -8083,9 +8141,9 @@
       <c r="A44" s="28">
         <v>43</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="32" t="s">
         <v>94</v>
       </c>
@@ -8103,9 +8161,9 @@
       <c r="A45" s="28">
         <v>44</v>
       </c>
-      <c r="B45" s="41"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="32" t="s">
         <v>95</v>
       </c>
@@ -8123,11 +8181,11 @@
       <c r="A46" s="28">
         <v>45</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="39" t="s">
+      <c r="B46" s="38"/>
+      <c r="C46" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="39" t="s">
+      <c r="D46" s="37" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -8147,9 +8205,9 @@
       <c r="A47" s="28">
         <v>46</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
       <c r="E47" s="4" t="s">
         <v>45</v>
       </c>
@@ -8167,9 +8225,9 @@
       <c r="A48" s="28">
         <v>47</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
       <c r="E48" s="4" t="s">
         <v>42</v>
       </c>
@@ -8187,9 +8245,9 @@
       <c r="A49" s="28">
         <v>48</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
       <c r="E49" s="4" t="s">
         <v>43</v>
       </c>
@@ -8207,9 +8265,9 @@
       <c r="A50" s="28">
         <v>49</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
       <c r="E50" s="4" t="s">
         <v>46</v>
       </c>
@@ -8227,9 +8285,9 @@
       <c r="A51" s="28">
         <v>50</v>
       </c>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="40"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="39"/>
       <c r="E51" s="4" t="s">
         <v>44</v>
       </c>
@@ -8247,9 +8305,9 @@
       <c r="A52" s="28">
         <v>51</v>
       </c>
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="39" t="s">
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="37" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="4" t="s">
@@ -8269,9 +8327,9 @@
       <c r="A53" s="28">
         <v>52</v>
       </c>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
       <c r="E53" s="4" t="s">
         <v>45</v>
       </c>
@@ -8289,9 +8347,9 @@
       <c r="A54" s="28">
         <v>53</v>
       </c>
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
       <c r="E54" s="4" t="s">
         <v>42</v>
       </c>
@@ -8309,9 +8367,9 @@
       <c r="A55" s="28">
         <v>54</v>
       </c>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
       <c r="E55" s="4" t="s">
         <v>43</v>
       </c>
@@ -8329,9 +8387,9 @@
       <c r="A56" s="28">
         <v>55</v>
       </c>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
       <c r="E56" s="4" t="s">
         <v>46</v>
       </c>
@@ -8349,9 +8407,9 @@
       <c r="A57" s="28">
         <v>56</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
       <c r="E57" s="4" t="s">
         <v>44</v>
       </c>
@@ -8367,6 +8425,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B30:B57"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C46:C57"/>
+    <mergeCell ref="D46:D51"/>
+    <mergeCell ref="D52:D57"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="C42:C45"/>
     <mergeCell ref="B2:B29"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D6"/>
@@ -8378,17 +8447,6 @@
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B30:B57"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C46:C57"/>
-    <mergeCell ref="D46:D51"/>
-    <mergeCell ref="D52:D57"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="C42:C45"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D30 C38:D38 D52:D55 C46:D49 D35">
     <cfRule type="expression" dxfId="7" priority="8">

</xml_diff>